<commit_message>
Mise à jour du planning
</commit_message>
<xml_diff>
--- a/Rendus/Planning.xlsx
+++ b/Rendus/Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cours\TER_Art\Rendus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CD27DCC-4A16-45FB-8DB4-127F23A73A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2367DD8-3E9A-4774-8E47-175FE3938736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{333515FF-309C-4E44-8A4C-BE0A520770E0}"/>
   </bookViews>
@@ -35,22 +35,194 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>François Verdelhan</author>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{479055D9-969B-4380-8661-23D944896496}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+01/10 : Question de recherche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{7D16F124-D7B3-44F4-801E-DEFCD07D2C07}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+15/10 : Planning</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{E52E05E8-7037-4AF0-BC51-316A941A298F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+01/11 : Mise en forme et AED</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{0403FDDD-2844-4F90-B7BF-5953A9DD53F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+15/11 : Revue littérature</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="0" shapeId="0" xr:uid="{E5A6C526-7477-443F-9B9A-87561DFF4AE1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+01/12 : Outils et programmes à utiliser</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{5759B1EA-E166-4F77-8BD3-982C926500DD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+14/12 : Rendu slide pour présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P13" authorId="0" shapeId="0" xr:uid="{9024F7E2-CFC6-47C7-962A-C13DAC041746}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>François Verdelhan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rendu attendu :
+Présentation du contexte
+Ebauche du site
+Présentation de 2 modèles</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Semaine</t>
   </si>
   <si>
-    <t>Entrer en cour</t>
-  </si>
-  <si>
     <t>Rencontre avec l'interlocuteur</t>
-  </si>
-  <si>
-    <t>Plannification des taches</t>
-  </si>
-  <si>
-    <t>Nettoyage base de données</t>
   </si>
   <si>
     <t>Création du site</t>
@@ -59,29 +231,50 @@
     <t>Création des modèles</t>
   </si>
   <si>
-    <t>Selection du modèle</t>
-  </si>
-  <si>
     <t>Intégration des données au site</t>
   </si>
   <si>
     <t>Prise en main de la bibliographie</t>
   </si>
   <si>
-    <t>Présentation de mis semestre</t>
+    <t xml:space="preserve">Semaine de compte rendu </t>
   </si>
   <si>
-    <t>Présentation final</t>
+    <t>Entrée en cours</t>
   </si>
   <si>
-    <t xml:space="preserve">Semaine de compte rendu </t>
+    <t>Plannification des tâches</t>
+  </si>
+  <si>
+    <t>Sélection du modèle</t>
+  </si>
+  <si>
+    <t>Présentation de mi-semestre</t>
+  </si>
+  <si>
+    <t>Présentation finale</t>
+  </si>
+  <si>
+    <t>Ajout de module sur le site</t>
+  </si>
+  <si>
+    <t>Prévu</t>
+  </si>
+  <si>
+    <t>Retard</t>
+  </si>
+  <si>
+    <t>Nettoyage/Import base de données</t>
+  </si>
+  <si>
+    <t>Semaine de présentation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,8 +288,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,8 +315,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -149,13 +373,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -167,6 +421,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -182,7 +451,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -197,6 +466,21 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -331,6 +615,43 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -346,25 +667,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,6 +730,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,260 +1032,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D90E078-9C52-45F7-9223-E31D19317A62}">
-  <dimension ref="A2:AP15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D90E078-9C52-45F7-9223-E31D19317A62}">
+  <dimension ref="A1:AP17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="43" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="24"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="27"/>
+    </row>
+    <row r="3" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="26"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8">
+        <v>36</v>
+      </c>
+      <c r="C5" s="7">
+        <v>37</v>
+      </c>
+      <c r="D5" s="7">
+        <v>38</v>
+      </c>
+      <c r="E5" s="16">
+        <v>39</v>
+      </c>
+      <c r="F5" s="7">
+        <v>40</v>
+      </c>
+      <c r="G5" s="16">
+        <v>41</v>
+      </c>
+      <c r="H5" s="7">
+        <v>42</v>
+      </c>
+      <c r="I5" s="31">
+        <v>43</v>
+      </c>
+      <c r="J5" s="16">
+        <v>44</v>
+      </c>
+      <c r="K5" s="31">
+        <v>45</v>
+      </c>
+      <c r="L5" s="16">
+        <v>46</v>
+      </c>
+      <c r="M5" s="31">
+        <v>47</v>
+      </c>
+      <c r="N5" s="16">
+        <v>48</v>
+      </c>
+      <c r="O5" s="31">
+        <v>49</v>
+      </c>
+      <c r="P5" s="33">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="31">
+        <v>51</v>
+      </c>
+      <c r="R5" s="31">
+        <v>52</v>
+      </c>
+      <c r="S5" s="31">
+        <v>1</v>
+      </c>
+      <c r="T5" s="31">
+        <v>2</v>
+      </c>
+      <c r="U5" s="31">
+        <v>3</v>
+      </c>
+      <c r="V5" s="31">
+        <v>4</v>
+      </c>
+      <c r="W5" s="31">
+        <v>5</v>
+      </c>
+      <c r="X5" s="31">
+        <v>6</v>
+      </c>
+      <c r="Y5" s="31">
+        <v>7</v>
+      </c>
+      <c r="Z5" s="31">
+        <v>8</v>
+      </c>
+      <c r="AA5" s="31">
+        <v>9</v>
+      </c>
+      <c r="AB5" s="31">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="31">
+        <v>11</v>
+      </c>
+      <c r="AD5" s="31">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="10">
-        <v>36</v>
-      </c>
-      <c r="C4" s="8">
-        <v>37</v>
-      </c>
-      <c r="D4" s="8">
-        <v>38</v>
-      </c>
-      <c r="E4" s="8">
-        <v>39</v>
-      </c>
-      <c r="F4" s="8">
-        <v>40</v>
-      </c>
-      <c r="G4" s="8">
-        <v>41</v>
-      </c>
-      <c r="H4" s="8">
-        <v>42</v>
-      </c>
-      <c r="I4" s="8">
-        <v>43</v>
-      </c>
-      <c r="J4" s="8">
-        <v>44</v>
-      </c>
-      <c r="K4" s="8">
-        <v>45</v>
-      </c>
-      <c r="L4" s="8">
-        <v>46</v>
-      </c>
-      <c r="M4" s="8">
-        <v>47</v>
-      </c>
-      <c r="N4" s="8">
-        <v>48</v>
-      </c>
-      <c r="O4" s="8">
-        <v>49</v>
-      </c>
-      <c r="P4" s="8">
-        <v>50</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>51</v>
-      </c>
-      <c r="R4" s="8">
-        <v>52</v>
-      </c>
-      <c r="S4" s="8">
-        <v>1</v>
-      </c>
-      <c r="T4" s="8">
-        <v>2</v>
-      </c>
-      <c r="U4" s="8">
-        <v>3</v>
-      </c>
-      <c r="V4" s="8">
-        <v>4</v>
-      </c>
-      <c r="W4" s="8">
-        <v>5</v>
-      </c>
-      <c r="X4" s="8">
-        <v>6</v>
-      </c>
-      <c r="Y4" s="8">
-        <v>7</v>
-      </c>
-      <c r="Z4" s="8">
-        <v>8</v>
-      </c>
-      <c r="AA4" s="8">
-        <v>9</v>
-      </c>
-      <c r="AB4" s="8">
-        <v>10</v>
-      </c>
-      <c r="AC4" s="8">
-        <v>11</v>
-      </c>
-      <c r="AD4" s="8">
-        <v>12</v>
-      </c>
-      <c r="AE4" s="8">
+      <c r="AE5" s="31">
         <v>13</v>
       </c>
-      <c r="AF4" s="8">
+      <c r="AF5" s="31">
         <v>14</v>
       </c>
-      <c r="AG4" s="8">
+      <c r="AG5" s="31">
         <v>15</v>
       </c>
-      <c r="AH4" s="8">
+      <c r="AH5" s="31">
         <v>16</v>
       </c>
-      <c r="AI4" s="8">
+      <c r="AI5" s="31">
         <v>17</v>
       </c>
-      <c r="AJ4" s="8">
+      <c r="AJ5" s="31">
         <v>18</v>
       </c>
-      <c r="AK4" s="8">
+      <c r="AK5" s="31">
         <v>19</v>
       </c>
-      <c r="AL4" s="8">
+      <c r="AL5" s="31">
         <v>20</v>
       </c>
-      <c r="AM4" s="8">
+      <c r="AM5" s="31">
         <v>21</v>
       </c>
-      <c r="AN4" s="8">
+      <c r="AN5" s="31">
         <v>22</v>
       </c>
-      <c r="AO4" s="8">
+      <c r="AO5" s="31">
         <v>23</v>
       </c>
-      <c r="AP4" s="9">
+      <c r="AP5" s="32">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="6"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="6"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
-      <c r="AJ5" s="6"/>
-      <c r="AK5" s="6"/>
-      <c r="AL5" s="6"/>
-      <c r="AM5" s="6"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="6"/>
-      <c r="AP5" s="7"/>
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="2"/>
-      <c r="AE6" s="2"/>
-      <c r="AF6" s="2"/>
-      <c r="AG6" s="2"/>
-      <c r="AH6" s="2"/>
-      <c r="AI6" s="2"/>
-      <c r="AJ6" s="2"/>
-      <c r="AK6" s="2"/>
-      <c r="AL6" s="2"/>
-      <c r="AM6" s="2"/>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
-      <c r="AP6" s="3"/>
+      <c r="A6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="6"/>
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="12"/>
+      <c r="A7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -967,17 +1293,17 @@
       <c r="AP7" s="3"/>
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="12"/>
+      <c r="A8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1013,15 +1339,15 @@
       <c r="AP8" s="3"/>
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="12"/>
+      <c r="A9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1059,19 +1385,19 @@
       <c r="AP9" s="3"/>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="12"/>
+      <c r="A10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -1105,36 +1431,36 @@
       <c r="AP10" s="3"/>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="12"/>
+      <c r="A11" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2"/>
-      <c r="AB11" s="2"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
@@ -1151,10 +1477,10 @@
       <c r="AP11" s="3"/>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="12"/>
+      <c r="A12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="9"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1164,23 +1490,23 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="2"/>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
@@ -1197,10 +1523,10 @@
       <c r="AP12" s="3"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="12"/>
+      <c r="A13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="9"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1214,7 +1540,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="P13" s="19"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1243,10 +1569,10 @@
       <c r="AP13" s="3"/>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="12"/>
+      <c r="A14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="9"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1267,12 +1593,12 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="2"/>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="19"/>
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
@@ -1288,54 +1614,151 @@
       <c r="AO14" s="2"/>
       <c r="AP14" s="3"/>
     </row>
-    <row r="15" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="19"/>
+      <c r="AH15" s="19"/>
+      <c r="AI15" s="19"/>
+      <c r="AJ15" s="19"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="3"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="19"/>
+      <c r="AL16" s="19"/>
+      <c r="AM16" s="19"/>
+      <c r="AN16" s="19"/>
+      <c r="AO16" s="2"/>
+      <c r="AP16" s="3"/>
+    </row>
+    <row r="17" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
-      <c r="AG15" s="4"/>
-      <c r="AH15" s="4"/>
-      <c r="AI15" s="4"/>
-      <c r="AJ15" s="4"/>
-      <c r="AK15" s="4"/>
-      <c r="AL15" s="4"/>
-      <c r="AM15" s="4"/>
-      <c r="AN15" s="4"/>
-      <c r="AO15" s="4"/>
-      <c r="AP15" s="5"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+      <c r="AA17" s="4"/>
+      <c r="AB17" s="4"/>
+      <c r="AC17" s="4"/>
+      <c r="AD17" s="4"/>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+      <c r="AG17" s="4"/>
+      <c r="AH17" s="4"/>
+      <c r="AI17" s="4"/>
+      <c r="AJ17" s="4"/>
+      <c r="AK17" s="4"/>
+      <c r="AL17" s="4"/>
+      <c r="AM17" s="4"/>
+      <c r="AN17" s="4"/>
+      <c r="AO17" s="4"/>
+      <c r="AP17" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>